<commit_message>
rebuild to get pages working again
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-CmsInteroperabilityPolicyCodes.xlsx
+++ b/docs/CodeSystem-CmsInteroperabilityPolicyCodes.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.2.1</t>
+    <t>0.2.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-08-09T03:19:35-05:00</t>
+    <t>2024-09-11T16:17:59-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -66,7 +66,13 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>No display for ContactDetail</t>
+    <t>MITRE (https://www.mitre.org)</t>
+  </si>
+  <si>
+    <t>Jurisdiction</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Description</t>
@@ -305,7 +311,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -405,64 +411,72 @@
       <c r="A12" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" t="s" s="2">
+        <v>21</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="B19" t="s" s="2">
         <v>28</v>
       </c>
+      <c r="B19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
         <v>29</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" t="s" s="2">
+        <v>30</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>30</v>
-      </c>
-      <c r="B21" t="s" s="2">
         <v>31</v>
+      </c>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s" s="2">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -480,111 +494,111 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D9" s="2"/>
     </row>

</xml_diff>